<commit_message>
Added wf to delete a file if it exists; GenerateOutputCompanii file working and tested.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/UiPath/orange-payment-mix-calculation/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/POCs/Orange/Repo/orange-payment-mix-calculation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E1642B9-1546-4C88-B917-F4258B6D522C}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF03BDA9-4BBF-45EE-A08D-8BA0FBCE3AAD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>TARIFAR INCADRARE,REALIZAT SUPLIMENTAR,ORE DE NOAPTE,SPOR DE NOAPTE,PARTE VARIABILA NET,PRIMA DETASARE NET,NET PRIMA DE POST NET,PRIMA DE POST,PRIMA DE POST BRUT,PRIMA EXCEPTIONALA NET,PRIMA EXPATRIERE NET,PRIMA INTERIMAT NET,PRIMA MOBILITATE NET,PRIMA DETASARE BRUT,PRIMA OBISNUITA NETA,Regularizari Net,BONUS,PRIMA BRUTA ONCALL,PRIMA BRUTA OVERTIME,BENEFICIU IN NATURA,BRUT PT IMPOZITARE,BAZA CALCUL SOMAJ 1,BAZA CALCUL CAS,BAZA SANATATE,VENIT NET PT IMPOZITARE,BAZA PT IMPOZITARE,BRUT TICHETE MASA,BRUT TOTAL TICHETE,NET,CONTRIBUTIE SCHEMA PENSII,BRUT DIURNA DELEGATIE</t>
+  </si>
+  <si>
+    <t>Data\Output\companii.xlsx</t>
+  </si>
+  <si>
+    <t>Location to save the file "companii"</t>
+  </si>
+  <si>
+    <t>companiiFilePath</t>
   </si>
 </sst>
 </file>
@@ -557,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z994"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -654,19 +663,29 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="230.4">
-      <c r="A11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>49</v>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="230.4">
+      <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,6 +1667,8 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added workflows for MinMaxMed file calculation
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/POCs/Orange/Repo/orange-payment-mix-calculation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF03BDA9-4BBF-45EE-A08D-8BA0FBCE3AAD}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0F931C2-0FB2-4200-ADE9-B2FEEE43EB4C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>companiiFilePath</t>
+  </si>
+  <si>
+    <t>minMaxMedFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\MinMaxMed.xlsx</t>
+  </si>
+  <si>
+    <t>Location to save the file "MinMaxMed"</t>
   </si>
 </sst>
 </file>
@@ -566,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -674,19 +683,29 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="230.4">
-      <c r="A13" s="5" t="s">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="230.4">
+      <c r="A14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -1669,6 +1688,7 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>